<commit_message>
RR -> Piano di Progetto -> Completati diagrammi di gantt (tutti) e tabelle distrubuzione ore e ruoli per fase 1, 2 e 3
</commit_message>
<xml_diff>
--- a/RR/Esterni/Piano di Progetto/RISORSE_1_AN.xlsx
+++ b/RR/Esterni/Piano di Progetto/RISORSE_1_AN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
   <si>
     <t>Task Code</t>
   </si>
@@ -121,6 +121,51 @@
   </si>
   <si>
     <t>AN 5.2</t>
+  </si>
+  <si>
+    <t>Membro</t>
+  </si>
+  <si>
+    <t>I Periodo</t>
+  </si>
+  <si>
+    <t>II Periodo</t>
+  </si>
+  <si>
+    <t>Ore</t>
+  </si>
+  <si>
+    <t>Fase</t>
+  </si>
+  <si>
+    <t>Begolo Marco</t>
+  </si>
+  <si>
+    <t>Facchin Gabriele</t>
+  </si>
+  <si>
+    <t>Cornaglia Alessando</t>
+  </si>
+  <si>
+    <t>tutte</t>
+  </si>
+  <si>
+    <t>Dalla Pietà Massimo</t>
+  </si>
+  <si>
+    <t>Braghetto Lorenzo</t>
+  </si>
+  <si>
+    <t>Quadrio Giacomo</t>
+  </si>
+  <si>
+    <t>Maggiolo Giorgio</t>
+  </si>
+  <si>
+    <t>AN 1, 4.1, 4.2</t>
+  </si>
+  <si>
+    <t>AN 1, 4.3, 5.1</t>
   </si>
 </sst>
 </file>
@@ -160,7 +205,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -293,11 +338,248 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -318,6 +600,54 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -612,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M145"/>
+  <dimension ref="A1:U145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -630,9 +960,12 @@
     <col min="11" max="11" width="18.85546875" customWidth="1"/>
     <col min="12" max="12" width="19.85546875" customWidth="1"/>
     <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="15" max="15" width="21" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -667,7 +1000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:21">
       <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
@@ -678,7 +1011,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F2">
         <f>IF($C2="Responsabile",$D2,0)</f>
@@ -690,7 +1023,7 @@
       </c>
       <c r="H2">
         <f>IF($C2="Analista",$D2,0)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I2">
         <f>IF($C2="Verificatore",$D2,0)</f>
@@ -701,21 +1034,34 @@
       </c>
       <c r="L2" s="2">
         <f>SUM(F2:F109)</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M2" s="2">
         <f>L2</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>23</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="39"/>
+      <c r="U2" s="40"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1">
       <c r="A3" s="14"/>
       <c r="B3" s="5"/>
       <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F66" si="0">IF($C3="Responsabile",$D3,0)</f>
@@ -731,7 +1077,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I66" si="3">IF($C3="Verificatore",$D3,0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>10</v>
@@ -744,8 +1090,27 @@
         <f>L3</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="O3" s="34"/>
+      <c r="P3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
@@ -785,8 +1150,29 @@
         <f>L4/3</f>
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="O4" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>13</v>
+      </c>
+      <c r="R4" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="S4" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4" s="23">
+        <v>10</v>
+      </c>
+      <c r="U4" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="14"/>
       <c r="B5" s="5"/>
       <c r="C5" s="14" t="s">
@@ -822,8 +1208,29 @@
         <f>L5/2</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="O5" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>11</v>
+      </c>
+      <c r="R5" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="21">
+        <v>8</v>
+      </c>
+      <c r="U5" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
@@ -853,8 +1260,29 @@
         <v>0</v>
       </c>
       <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="O6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="P6" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>11</v>
+      </c>
+      <c r="R6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" s="21">
+        <v>10</v>
+      </c>
+      <c r="U6" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="15"/>
       <c r="B7" s="3"/>
       <c r="C7" s="15" t="s">
@@ -879,8 +1307,29 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>11</v>
+      </c>
+      <c r="R7" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="S7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="21">
+        <v>8</v>
+      </c>
+      <c r="U7" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -891,11 +1340,11 @@
         <v>11</v>
       </c>
       <c r="D8" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
@@ -909,8 +1358,29 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="P8" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>10</v>
+      </c>
+      <c r="R8" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="S8" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="21">
+        <v>10</v>
+      </c>
+      <c r="U8" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" s="14"/>
       <c r="B9" s="5"/>
       <c r="C9" s="14" t="s">
@@ -935,8 +1405,29 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="O9" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="P9" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>10</v>
+      </c>
+      <c r="R9" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="21">
+        <v>10</v>
+      </c>
+      <c r="U9" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15.75" thickBot="1">
       <c r="A10" s="15" t="s">
         <v>30</v>
       </c>
@@ -965,8 +1456,29 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="29">
+        <v>10</v>
+      </c>
+      <c r="R10" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="S10" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="29">
+        <v>10</v>
+      </c>
+      <c r="U10" s="41" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" s="15"/>
       <c r="B11" s="3"/>
       <c r="C11" s="15" t="s">
@@ -991,8 +1503,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -1003,7 +1522,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="11">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
@@ -1015,14 +1534,21 @@
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="15" t="s">
         <v>32</v>
       </c>
@@ -1033,7 +1559,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
@@ -1049,10 +1575,17 @@
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>19</v>
+      </c>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="15"/>
       <c r="B14" s="3"/>
       <c r="C14" s="15" t="s">
@@ -1077,8 +1610,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -1092,23 +1632,30 @@
         <v>14</v>
       </c>
       <c r="F15">
-        <f>IF($C15="Responsabile",$D15,0)</f>
+        <f t="shared" ref="F15:F20" si="4">IF($C15="Responsabile",$D15,0)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>IF($C15="Amministratore",$D15,0)</f>
+        <f t="shared" ref="G15:G20" si="5">IF($C15="Amministratore",$D15,0)</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>IF($C15="Analista",$D15,0)</f>
+        <f t="shared" ref="H15:H20" si="6">IF($C15="Analista",$D15,0)</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>IF($C15="Verificatore",$D15,0)</f>
+        <f t="shared" ref="I15:I20" si="7">IF($C15="Verificatore",$D15,0)</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="15" t="s">
         <v>34</v>
       </c>
@@ -1122,23 +1669,30 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <f>IF($C16="Responsabile",$D16,0)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G16">
-        <f>IF($C16="Amministratore",$D16,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f>IF($C16="Analista",$D16,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>IF($C16="Verificatore",$D16,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="16" t="s">
         <v>29</v>
       </c>
@@ -1152,78 +1706,86 @@
         <v>5</v>
       </c>
       <c r="F17">
-        <f>IF($C17="Responsabile",$D17,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f>IF($C17="Amministratore",$D17,0)</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="H17">
-        <f>IF($C17="Analista",$D17,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I17">
-        <f>IF($C17="Verificatore",$D17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="3"/>
+    </row>
+    <row r="18" spans="1:21">
       <c r="F18">
-        <f>IF($C18="Responsabile",$D18,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G18">
-        <f>IF($C18="Amministratore",$D18,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f>IF($C18="Analista",$D18,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I18">
-        <f>IF($C18="Verificatore",$D18,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="43"/>
+    </row>
+    <row r="19" spans="1:21">
       <c r="C19" s="1"/>
       <c r="F19">
-        <f>IF($C19="Responsabile",$D19,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G19">
-        <f>IF($C19="Amministratore",$D19,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f>IF($C19="Analista",$D19,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I19">
-        <f>IF($C19="Verificatore",$D19,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
       <c r="F20">
-        <f>IF($C20="Responsabile",$D20,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G20">
-        <f>IF($C20="Amministratore",$D20,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H20">
-        <f>IF($C20="Analista",$D20,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I20">
-        <f>IF($C20="Verificatore",$D20,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
       <c r="F21">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1241,7 +1803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:21">
       <c r="F22">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1259,7 +1821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:21">
       <c r="F23">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1277,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:21">
       <c r="F24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1295,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:21">
       <c r="F25">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1313,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:21">
       <c r="F26">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1331,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:21">
       <c r="F27">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1349,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:21">
       <c r="F28">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1367,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:21">
       <c r="F29">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1385,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:21">
       <c r="F30">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1403,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:21">
       <c r="F31">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1421,7 +1983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:21">
       <c r="F32">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2053,1427 +2615,1432 @@
     </row>
     <row r="67" spans="6:9">
       <c r="F67">
-        <f t="shared" ref="F67:F130" si="4">IF($C67="Responsabile",$D67,0)</f>
+        <f t="shared" ref="F67:F130" si="8">IF($C67="Responsabile",$D67,0)</f>
         <v>0</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G130" si="5">IF($C67="Amministratore",$D67,0)</f>
+        <f t="shared" ref="G67:G130" si="9">IF($C67="Amministratore",$D67,0)</f>
         <v>0</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H130" si="6">IF($C67="Analista",$D67,0)</f>
+        <f t="shared" ref="H67:H130" si="10">IF($C67="Analista",$D67,0)</f>
         <v>0</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I130" si="7">IF($C67="Verificatore",$D67,0)</f>
+        <f t="shared" ref="I67:I130" si="11">IF($C67="Verificatore",$D67,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="6:9">
       <c r="F68">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="6:9">
       <c r="F69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="6:9">
       <c r="F70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="6:9">
       <c r="F71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="6:9">
       <c r="F72">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="6:9">
       <c r="F73">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="6:9">
       <c r="F74">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="6:9">
       <c r="F75">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="6:9">
       <c r="F76">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="6:9">
       <c r="F77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="6:9">
       <c r="F78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I78">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="79" spans="6:9">
       <c r="F79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I79">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="6:9">
       <c r="F80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I80">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="81" spans="6:9">
       <c r="F81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I81">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="82" spans="6:9">
       <c r="F82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I82">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="6:9">
       <c r="F83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I83">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="84" spans="6:9">
       <c r="F84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I84">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="6:9">
       <c r="F85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I85">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="6:9">
       <c r="F86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I86">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="6:9">
       <c r="F87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I87">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="88" spans="6:9">
       <c r="F88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I88">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="6:9">
       <c r="F89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="6:9">
       <c r="F90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I90">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="91" spans="6:9">
       <c r="F91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I91">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="6:9">
       <c r="F92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I92">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="6:9">
       <c r="F93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I93">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="6:9">
       <c r="F94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I94">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="95" spans="6:9">
       <c r="F95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I95">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="6:9">
       <c r="F96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I96">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="97" spans="6:9">
       <c r="F97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I97">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="98" spans="6:9">
       <c r="F98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I98">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="6:9">
       <c r="F99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I99">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="6:9">
       <c r="F100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I100">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="6:9">
       <c r="F101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I101">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="6:9">
       <c r="F102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I102">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="6:9">
       <c r="F103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H103">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I103">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="6:9">
       <c r="F104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H104">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I104">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="105" spans="6:9">
       <c r="F105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I105">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="6:9">
       <c r="F106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I106">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="107" spans="6:9">
       <c r="F107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I107">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="6:9">
       <c r="F108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I108">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="109" spans="6:9">
       <c r="F109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H109">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I109">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="110" spans="6:9">
       <c r="F110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H110">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I110">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="6:9">
       <c r="F111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I111">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="112" spans="6:9">
       <c r="F112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H112">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I112">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="6:9">
       <c r="F113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I113">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="114" spans="6:9">
       <c r="F114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G114">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H114">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I114">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="115" spans="6:9">
       <c r="F115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G115">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H115">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I115">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="6:9">
       <c r="F116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G116">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H116">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I116">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="6:9">
       <c r="F117">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G117">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H117">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I117">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="6:9">
       <c r="F118">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G118">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H118">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I118">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="6:9">
       <c r="F119">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G119">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H119">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I119">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="120" spans="6:9">
       <c r="F120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G120">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H120">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I120">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="6:9">
       <c r="F121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G121">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H121">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I121">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="122" spans="6:9">
       <c r="F122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G122">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H122">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I122">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="123" spans="6:9">
       <c r="F123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G123">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H123">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I123">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="6:9">
       <c r="F124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G124">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H124">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I124">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="6:9">
       <c r="F125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G125">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H125">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I125">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="6:9">
       <c r="F126">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G126">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H126">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I126">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="6:9">
       <c r="F127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G127">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H127">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I127">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="6:9">
       <c r="F128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G128">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H128">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I128">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="129" spans="6:9">
       <c r="F129">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G129">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H129">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I129">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="130" spans="6:9">
       <c r="F130">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G130">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H130">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="I130">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="6:9">
       <c r="F131">
-        <f t="shared" ref="F131:F145" si="8">IF($C131="Responsabile",$D131,0)</f>
+        <f t="shared" ref="F131:F145" si="12">IF($C131="Responsabile",$D131,0)</f>
         <v>0</v>
       </c>
       <c r="G131">
-        <f t="shared" ref="G131:G145" si="9">IF($C131="Amministratore",$D131,0)</f>
+        <f t="shared" ref="G131:G145" si="13">IF($C131="Amministratore",$D131,0)</f>
         <v>0</v>
       </c>
       <c r="H131">
-        <f t="shared" ref="H131:H145" si="10">IF($C131="Analista",$D131,0)</f>
+        <f t="shared" ref="H131:H145" si="14">IF($C131="Analista",$D131,0)</f>
         <v>0</v>
       </c>
       <c r="I131">
-        <f t="shared" ref="I131:I145" si="11">IF($C131="Verificatore",$D131,0)</f>
+        <f t="shared" ref="I131:I145" si="15">IF($C131="Verificatore",$D131,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="132" spans="6:9">
       <c r="F132">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G132">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H132">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I132">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="133" spans="6:9">
       <c r="F133">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G133">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H133">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I133">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="6:9">
       <c r="F134">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G134">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H134">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I134">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="135" spans="6:9">
       <c r="F135">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G135">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H135">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I135">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="136" spans="6:9">
       <c r="F136">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G136">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H136">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I136">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="137" spans="6:9">
       <c r="F137">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G137">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H137">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I137">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="138" spans="6:9">
       <c r="F138">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G138">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H138">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I138">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="139" spans="6:9">
       <c r="F139">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G139">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H139">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I139">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="140" spans="6:9">
       <c r="F140">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G140">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H140">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I140">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="6:9">
       <c r="F141">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G141">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H141">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I141">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="142" spans="6:9">
       <c r="F142">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G142">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H142">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I142">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="143" spans="6:9">
       <c r="F143">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G143">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H143">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I143">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="144" spans="6:9">
       <c r="F144">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G144">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H144">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I144">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
     <row r="145" spans="6:9">
       <c r="F145">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="G145">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="H145">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="I145">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:U2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
RR-> piano di progetto -> chiarite le sigle per i ruoli nel capitolo 2
</commit_message>
<xml_diff>
--- a/RR/Esterni/Piano di Progetto/RISORSE_1_AN.xlsx
+++ b/RR/Esterni/Piano di Progetto/RISORSE_1_AN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>Task Code</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Ore totali di lavoro</t>
   </si>
   <si>
-    <t>Ore di lavoro Cad.</t>
-  </si>
-  <si>
     <t>Stesura PQ</t>
   </si>
   <si>
@@ -169,12 +166,18 @@
   </si>
   <si>
     <t>Totale</t>
+  </si>
+  <si>
+    <t>Costo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -208,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -668,59 +671,98 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <top/>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -729,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -749,7 +791,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -794,11 +835,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -810,10 +854,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1108,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1123,25 +1178,26 @@
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" customWidth="1"/>
     <col min="8" max="9" width="3.28515625" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
-    <col min="12" max="12" width="19.85546875" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="14" max="14" width="83.42578125" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
     <col min="21" max="21" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A1" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
@@ -1156,18 +1212,18 @@
       <c r="I1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="45" t="s">
-        <v>25</v>
+      <c r="M1" s="44" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:22">
+      <c r="A2" s="31" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1176,7 +1232,7 @@
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="32">
         <v>6</v>
       </c>
       <c r="F2">
@@ -1195,38 +1251,44 @@
         <f>IF($C2="Verificatore",$D2,0)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="38" t="s">
         <v>11</v>
       </c>
       <c r="L2" s="1">
-        <f>SUM(F2:F109)</f>
-        <v>46</v>
-      </c>
-      <c r="M2" s="46">
-        <f>L2</f>
-        <v>46</v>
-      </c>
-      <c r="O2" s="51" t="s">
+        <f>SUM(F$2:F$17)</f>
+        <v>23</v>
+      </c>
+      <c r="M2" s="51">
+        <f>L2*N2</f>
+        <v>690</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="53" t="s">
+      <c r="Q2" s="56"/>
+      <c r="R2" s="57"/>
+      <c r="S2" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="54"/>
-      <c r="U2" s="55"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="53" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A3" s="34"/>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A3" s="33"/>
       <c r="B3" s="3"/>
       <c r="C3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="35">
+      <c r="D3" s="34">
         <v>3</v>
       </c>
       <c r="F3">
@@ -1245,39 +1307,43 @@
         <f t="shared" ref="I3:I14" si="3">IF($C3="Verificatore",$D3,0)</f>
         <v>3</v>
       </c>
-      <c r="K3" s="39" t="s">
+      <c r="K3" s="38" t="s">
         <v>10</v>
       </c>
       <c r="L3" s="1">
-        <f>SUM(G2:G110)</f>
-        <v>40</v>
-      </c>
-      <c r="M3" s="46">
-        <f>L3</f>
-        <v>40</v>
-      </c>
-      <c r="O3" s="52"/>
-      <c r="P3" s="23" t="s">
+        <f>SUM(G$2:G$17)</f>
+        <v>20</v>
+      </c>
+      <c r="M3" s="51">
+        <f t="shared" ref="M3:M5" si="4">L3*N3</f>
+        <v>400</v>
+      </c>
+      <c r="N3">
+        <v>20</v>
+      </c>
+      <c r="O3" s="54"/>
+      <c r="P3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="Q3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="R3" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="S3" s="23" t="s">
+      <c r="S3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="22" t="s">
+      <c r="T3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="24" t="s">
-        <v>39</v>
-      </c>
+      <c r="V3" s="66"/>
     </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:22">
+      <c r="A4" s="31" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -1286,7 +1352,7 @@
       <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="36">
+      <c r="D4" s="35">
         <v>10</v>
       </c>
       <c r="F4">
@@ -1305,19 +1371,22 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="K4" s="38" t="s">
         <v>6</v>
       </c>
       <c r="L4" s="1">
-        <f>SUM(H2:H111)</f>
-        <v>126</v>
-      </c>
-      <c r="M4" s="46">
-        <f>L4/3</f>
-        <v>42</v>
-      </c>
-      <c r="O4" s="19" t="s">
-        <v>40</v>
+        <f>SUM(H$2:H$17)</f>
+        <v>63</v>
+      </c>
+      <c r="M4" s="51">
+        <f t="shared" si="4"/>
+        <v>1575</v>
+      </c>
+      <c r="N4">
+        <v>25</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>39</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>20</v>
@@ -1325,8 +1394,8 @@
       <c r="Q4" s="12">
         <v>13</v>
       </c>
-      <c r="R4" s="26" t="s">
-        <v>43</v>
+      <c r="R4" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="S4" s="11" t="s">
         <v>22</v>
@@ -1334,17 +1403,21 @@
       <c r="T4" s="12">
         <v>10</v>
       </c>
-      <c r="U4" s="13" t="s">
-        <v>48</v>
+      <c r="U4" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" s="65">
+        <f>SUM(T4,Q4)</f>
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A5" s="34"/>
+    <row r="5" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A5" s="33"/>
       <c r="B5" s="3"/>
       <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="35">
+      <c r="D5" s="34">
         <v>2</v>
       </c>
       <c r="F5">
@@ -1363,41 +1436,48 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K5" s="32" t="s">
+      <c r="K5" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="6">
-        <f>SUM(I2:I112)</f>
-        <v>72</v>
-      </c>
-      <c r="M5" s="56">
-        <f>L5/2</f>
+      <c r="L5" s="1">
+        <f>SUM(I$2:I$17)</f>
         <v>36</v>
       </c>
-      <c r="O5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="P5" s="14" t="s">
+      <c r="M5" s="51">
+        <f t="shared" si="4"/>
+        <v>540</v>
+      </c>
+      <c r="N5">
+        <v>15</v>
+      </c>
+      <c r="O5" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" s="13" t="s">
         <v>22</v>
       </c>
       <c r="Q5" s="10">
         <v>11</v>
       </c>
-      <c r="R5" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="S5" s="14" t="s">
+      <c r="R5" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="13" t="s">
         <v>23</v>
       </c>
       <c r="T5" s="10">
         <v>8</v>
       </c>
-      <c r="U5" s="15" t="s">
-        <v>49</v>
+      <c r="U5" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="V5" s="63">
+        <f t="shared" ref="V5:V10" si="5">SUM(T5,Q5)</f>
+        <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A6" s="37" t="s">
+    <row r="6" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A6" s="36" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1406,7 +1486,7 @@
       <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="37">
         <v>6</v>
       </c>
       <c r="F6">
@@ -1425,43 +1505,50 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K6" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="58">
+      <c r="K6" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="L6" s="50">
         <f>SUM(L2:L5)</f>
-        <v>284</v>
-      </c>
-      <c r="M6" s="59"/>
-      <c r="O6" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="M6" s="52">
+        <f>SUM(M2:M5)</f>
+        <v>3205</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="13" t="s">
         <v>22</v>
       </c>
       <c r="Q6" s="10">
         <v>11</v>
       </c>
-      <c r="R6" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="S6" s="14" t="s">
+      <c r="R6" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="13" t="s">
         <v>21</v>
       </c>
       <c r="T6" s="10">
         <v>10</v>
       </c>
-      <c r="U6" s="16" t="s">
-        <v>43</v>
+      <c r="U6" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" s="63">
+        <f t="shared" si="5"/>
+        <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="37"/>
+    <row r="7" spans="1:22">
+      <c r="A7" s="36"/>
       <c r="B7" s="2"/>
       <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="37">
         <v>2</v>
       </c>
       <c r="F7">
@@ -1480,30 +1567,34 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O7" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="P7" s="14" t="s">
+      <c r="O7" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="13" t="s">
         <v>22</v>
       </c>
       <c r="Q7" s="10">
         <v>11</v>
       </c>
-      <c r="R7" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="S7" s="14" t="s">
+      <c r="R7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" s="13" t="s">
         <v>23</v>
       </c>
       <c r="T7" s="10">
         <v>8</v>
       </c>
-      <c r="U7" s="15" t="s">
-        <v>49</v>
+      <c r="U7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="V7" s="63">
+        <f t="shared" si="5"/>
+        <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:22">
+      <c r="A8" s="31" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1512,7 +1603,7 @@
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="35">
         <v>8</v>
       </c>
       <c r="F8">
@@ -1531,35 +1622,39 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O8" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="P8" s="14" t="s">
+      <c r="O8" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="13" t="s">
         <v>23</v>
       </c>
       <c r="Q8" s="10">
         <v>10</v>
       </c>
-      <c r="R8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="S8" s="14" t="s">
+      <c r="R8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="S8" s="13" t="s">
         <v>22</v>
       </c>
       <c r="T8" s="10">
         <v>10</v>
       </c>
-      <c r="U8" s="15" t="s">
-        <v>48</v>
+      <c r="U8" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="V8" s="63">
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="34"/>
+    <row r="9" spans="1:22">
+      <c r="A9" s="33"/>
       <c r="B9" s="3"/>
       <c r="C9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="34">
         <v>3</v>
       </c>
       <c r="F9">
@@ -1578,31 +1673,35 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O9" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" s="14" t="s">
+      <c r="O9" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="P9" s="13" t="s">
         <v>21</v>
       </c>
       <c r="Q9" s="10">
         <v>10</v>
       </c>
-      <c r="R9" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="S9" s="14" t="s">
+      <c r="R9" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="S9" s="13" t="s">
         <v>20</v>
       </c>
       <c r="T9" s="10">
         <v>10</v>
       </c>
-      <c r="U9" s="16" t="s">
-        <v>43</v>
+      <c r="U9" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="V9" s="63">
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A10" s="37" t="s">
-        <v>30</v>
+    <row r="10" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A10" s="36" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>16</v>
@@ -1610,7 +1709,7 @@
       <c r="C10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="37">
         <v>1</v>
       </c>
       <c r="F10">
@@ -1629,35 +1728,39 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O10" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="P10" s="17" t="s">
+      <c r="O10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="P10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="Q10" s="18">
+      <c r="Q10" s="17">
         <v>10</v>
       </c>
-      <c r="R10" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="17" t="s">
+      <c r="R10" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="18">
+      <c r="T10" s="17">
         <v>10</v>
       </c>
-      <c r="U10" s="25" t="s">
-        <v>48</v>
+      <c r="U10" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="V10" s="64">
+        <f t="shared" si="5"/>
+        <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="37"/>
+    <row r="11" spans="1:22">
+      <c r="A11" s="36"/>
       <c r="B11" s="2"/>
       <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="37">
         <v>1</v>
       </c>
       <c r="F11">
@@ -1684,9 +1787,9 @@
       <c r="T11" s="9"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="39" t="s">
-        <v>31</v>
+    <row r="12" spans="1:22">
+      <c r="A12" s="38" t="s">
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>17</v>
@@ -1694,7 +1797,7 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="39">
         <v>56</v>
       </c>
       <c r="F12">
@@ -1721,9 +1824,9 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="37" t="s">
-        <v>32</v>
+    <row r="13" spans="1:22">
+      <c r="A13" s="36" t="s">
+        <v>31</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>18</v>
@@ -1731,7 +1834,7 @@
       <c r="C13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="37">
         <v>19</v>
       </c>
       <c r="F13">
@@ -1758,13 +1861,13 @@
       <c r="T13" s="9"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="37"/>
+    <row r="14" spans="1:22">
+      <c r="A14" s="36"/>
       <c r="B14" s="2"/>
       <c r="C14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="37">
         <v>4</v>
       </c>
       <c r="F14">
@@ -1791,33 +1894,33 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="39" t="s">
-        <v>33</v>
+    <row r="15" spans="1:22">
+      <c r="A15" s="38" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="39">
         <v>14</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F17" si="4">IF($C15="Responsabile",$D15,0)</f>
+        <f t="shared" ref="F15:F17" si="6">IF($C15="Responsabile",$D15,0)</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15:G17" si="5">IF($C15="Amministratore",$D15,0)</f>
+        <f t="shared" ref="G15:G17" si="7">IF($C15="Amministratore",$D15,0)</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H17" si="6">IF($C15="Analista",$D15,0)</f>
+        <f t="shared" ref="H15:H17" si="8">IF($C15="Analista",$D15,0)</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="I15:I17" si="7">IF($C15="Verificatore",$D15,0)</f>
+        <f t="shared" ref="I15:I17" si="9">IF($C15="Verificatore",$D15,0)</f>
         <v>14</v>
       </c>
       <c r="O15" s="2"/>
@@ -1828,33 +1931,33 @@
       <c r="T15" s="9"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="37" t="s">
-        <v>34</v>
+    <row r="16" spans="1:22">
+      <c r="A16" s="36" t="s">
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="38">
+      <c r="D16" s="37">
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O16" s="2"/>
@@ -1866,32 +1969,32 @@
       <c r="U16" s="2"/>
     </row>
     <row r="17" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A17" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="42" t="s">
+      <c r="A17" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="B17" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="43">
         <v>5</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="H17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O17" s="2"/>
@@ -1903,15 +2006,15 @@
       <c r="U17" s="2"/>
     </row>
     <row r="18" spans="1:21" ht="15.75" thickBot="1">
-      <c r="O18" s="27"/>
+      <c r="O18" s="26"/>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1">
-      <c r="A19" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="48"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="50">
+      <c r="A19" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48">
         <f>SUM(D2:D17)</f>
         <v>142</v>
       </c>
@@ -1920,26 +2023,27 @@
         <v>23</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:I19" si="8">SUM(G2:G17)</f>
+        <f t="shared" ref="G19:I19" si="10">SUM(G2:G17)</f>
         <v>20</v>
       </c>
       <c r="H19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>63</v>
       </c>
       <c r="I19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>36</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="P2:R2"/>
     <mergeCell ref="S2:U2"/>
+    <mergeCell ref="V2:V3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>